<commit_message>
Added new Queries FC & EC
</commit_message>
<xml_diff>
--- a/Calculator2.8/ECData.xlsx
+++ b/Calculator2.8/ECData.xlsx
@@ -26,10 +26,10 @@
     <t>EC Summary</t>
   </si>
   <si>
-    <t>127977138182</t>
+    <t>008994670063</t>
   </si>
   <si>
-    <t>602.25</t>
+    <t>229.95</t>
   </si>
 </sst>
 </file>

</xml_diff>